<commit_message>
finished patient module and health insurance module mapping
</commit_message>
<xml_diff>
--- a/mapping/mml_health_insurance_mapping.xlsx
+++ b/mapping/mml_health_insurance_mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="307">
   <si>
     <t>MML</t>
     <phoneticPr fontId="1"/>
@@ -1565,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B109" workbookViewId="0">
-      <selection activeCell="K134" sqref="K134"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="K71" sqref="K71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3003,6 +3003,9 @@
       </c>
       <c r="I71" s="6" t="s">
         <v>144</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>211</v>
       </c>
       <c r="K71" t="s">
         <v>256</v>

</xml_diff>